<commit_message>
with correct css position(app.css included)
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R0ea95eef2d0143f4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R347d77391cfc4807"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0c1789a691394932"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R48f9179a8ff24e36"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{55dd97a7-9c7c-498d-bd98-68d191398d4f}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{66afaa3d-7f3b-499e-8759-81dfb996fa3b}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
merge app.js into interactivesdk.js worked! two apps working together now!
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R347d77391cfc4807"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R0f572b2d703b4631"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R48f9179a8ff24e36"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5cdb681588274851"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{66afaa3d-7f3b-499e-8759-81dfb996fa3b}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{309fb003-01db-47cc-844e-a75d414c63ff}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
code snippet show up after click goButton
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R0f572b2d703b4631"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb09f75b7f8a64ac1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5cdb681588274851"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8dc7026e30254bea"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{309fb003-01db-47cc-844e-a75d414c63ff}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{cdcaf53f-0393-45ed-be89-bbe42a35b019}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
add menu of navi back to main
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb09f75b7f8a64ac1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6cb4db02091b415b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8dc7026e30254bea"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R495185dd37fd47e7"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{cdcaf53f-0393-45ed-be89-bbe42a35b019}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e38bc884-8ad8-4141-86e5-913ed5ecf4bb}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
empty select second time, will show empty code
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2dfc38de9296460d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R718857f9b7264b06"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4c6ea3fabc3644ef"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9b5ce9fc3b5d4890"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{eb1eed8f-159b-4dc3-923e-afb67422675f}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2f7c5c6d-3474-418b-9f05-15841bb3c977}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
change api tutorial menu
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R718857f9b7264b06"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb3063feb32094a19"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9b5ce9fc3b5d4890"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd3e2d18c0f2142ca"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2f7c5c6d-3474-418b-9f05-15841bb3c977}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ee7f7073-9eb9-47bd-bce1-68ee03cb9e4c}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
can work in word, excel. powerpoint desktop
</commit_message>
<xml_diff>
--- a/OfficeApp3/bin/Debug/Book1.xlsx
+++ b/OfficeApp3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb3063feb32094a19"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re4fa753ae3f648d4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd3e2d18c0f2142ca"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R6adc00e236b14b71"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ee7f7073-9eb9-47bd-bce1-68ee03cb9e4c}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{00a9b675-660b-4e00-9aaa-6050dd764d23}">
   <we:reference id="2e33f014-880f-473a-870b-1f9fa5cacdfe" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>